<commit_message>
add parse for update schedule
</commit_message>
<xml_diff>
--- a/static/schedule/Pасписание/1 марта 2024 пятница.xlsx
+++ b/static/schedule/Pасписание/1 марта 2024 пятница.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="113">
   <si>
     <t>Согласовано:</t>
   </si>
@@ -223,10 +223,6 @@
 Берендеева О.С.</t>
   </si>
   <si>
-    <t xml:space="preserve">1 марта 2024 (пятница) 
-</t>
-  </si>
-  <si>
     <t>Правовое обеспечение профессиональной деятельности
 Кабанов А.Ю.</t>
   </si>
@@ -284,10 +280,6 @@
 Берендеева О.С</t>
   </si>
   <si>
-    <t>Иностранный язык
-Коротина М.А.</t>
-  </si>
-  <si>
     <t>Основы социологии и политологии
 Панов О.А.</t>
   </si>
@@ -400,6 +392,24 @@
   <si>
     <t>Иностранный язык 
 Иванова Е.В.</t>
+  </si>
+  <si>
+    <t>Иностранный язык
+Диф зачет
+Коротина М.А.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 марта 2024 (пятница) </t>
+  </si>
+  <si>
+    <t>Математическое моделирование 
+Самостоятельная работа
+Галямов Я.М.</t>
+  </si>
+  <si>
+    <t>Разработка программного обеспечения для мобильных устройств
+Самостоятельная работа
+Горелов А.С.</t>
   </si>
 </sst>
 </file>
@@ -1651,8 +1661,8 @@
   </sheetPr>
   <dimension ref="A1:T54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1690,7 +1700,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="66" t="s">
-        <v>61</v>
+        <v>110</v>
       </c>
       <c r="C1" s="66"/>
       <c r="D1" s="66"/>
@@ -1760,21 +1770,21 @@
         <v>48</v>
       </c>
       <c r="F3" s="33" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G3" s="45" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H3" s="27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I3" s="45"/>
       <c r="J3" s="39"/>
       <c r="K3" s="48" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L3" s="27" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="M3" s="45"/>
       <c r="N3" s="33" t="s">
@@ -1795,16 +1805,16 @@
       <c r="C4" s="50"/>
       <c r="D4" s="33"/>
       <c r="E4" s="50" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F4" s="33" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G4" s="21" t="s">
         <v>46</v>
       </c>
       <c r="H4" s="33" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I4" s="45"/>
       <c r="J4" s="33"/>
@@ -1812,13 +1822,13 @@
         <v>47</v>
       </c>
       <c r="L4" s="33" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="M4" s="48" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N4" s="27" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="O4" s="48"/>
       <c r="P4" s="33"/>
@@ -1826,7 +1836,7 @@
         <v>55</v>
       </c>
       <c r="R4" s="27" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="71.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1846,31 +1856,31 @@
         <v>46</v>
       </c>
       <c r="J5" s="33" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K5" s="48" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L5" s="27" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="M5" s="48" t="s">
         <v>47</v>
       </c>
       <c r="N5" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="O5" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="P5" s="33" t="s">
         <v>94</v>
-      </c>
-      <c r="O5" s="48" t="s">
-        <v>63</v>
-      </c>
-      <c r="P5" s="33" t="s">
-        <v>96</v>
       </c>
       <c r="Q5" s="21" t="s">
         <v>54</v>
       </c>
       <c r="R5" s="27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1884,41 +1894,41 @@
         <v>53</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E6" s="50"/>
       <c r="F6" s="33"/>
       <c r="G6" s="39"/>
       <c r="H6" s="34"/>
       <c r="I6" s="63" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J6" s="34" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K6" s="39" t="s">
         <v>37</v>
       </c>
       <c r="L6" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="M6" s="48" t="s">
+        <v>106</v>
+      </c>
+      <c r="N6" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="M6" s="48" t="s">
-        <v>108</v>
-      </c>
-      <c r="N6" s="33" t="s">
-        <v>95</v>
-      </c>
       <c r="O6" s="48" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P6" s="27" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="Q6" s="21" t="s">
         <v>46</v>
       </c>
       <c r="R6" s="27" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1929,10 +1939,10 @@
         <v>42</v>
       </c>
       <c r="C7" s="64" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D7" s="65" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E7" s="50"/>
       <c r="F7" s="33" t="s">
@@ -1944,21 +1954,21 @@
         <v>48</v>
       </c>
       <c r="J7" s="33" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K7" s="48"/>
       <c r="L7" s="20"/>
       <c r="M7" s="48" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N7" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="O7" s="48" t="s">
-        <v>108</v>
-      </c>
-      <c r="P7" s="33" t="s">
-        <v>95</v>
+        <v>105</v>
+      </c>
+      <c r="O7" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="P7" s="27" t="s">
+        <v>91</v>
       </c>
       <c r="Q7" s="64"/>
       <c r="R7" s="34" t="s">
@@ -1973,10 +1983,10 @@
         <v>43</v>
       </c>
       <c r="C8" s="45" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E8" s="50" t="s">
         <v>36</v>
@@ -1990,7 +2000,7 @@
         <v>37</v>
       </c>
       <c r="J8" s="34" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K8" s="63"/>
       <c r="L8" s="33"/>
@@ -2053,10 +2063,10 @@
       <c r="C10" s="45"/>
       <c r="D10" s="33"/>
       <c r="E10" s="45" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G10" s="48"/>
       <c r="H10" s="33"/>
@@ -2066,13 +2076,13 @@
         <v>46</v>
       </c>
       <c r="L10" s="33" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="M10" s="50" t="s">
         <v>50</v>
       </c>
       <c r="N10" s="49" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="O10" s="48"/>
       <c r="P10" s="33"/>
@@ -2095,16 +2105,16 @@
       <c r="C11" s="45"/>
       <c r="D11" s="33"/>
       <c r="E11" s="45" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F11" s="27" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G11" s="50" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H11" s="33" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I11" s="21"/>
       <c r="J11" s="33"/>
@@ -2112,21 +2122,21 @@
         <v>56</v>
       </c>
       <c r="L11" s="33" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="M11" s="45" t="s">
         <v>52</v>
       </c>
       <c r="N11" s="49" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="O11" s="48"/>
       <c r="P11" s="33"/>
       <c r="Q11" s="50" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="R11" s="33" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="S11" s="62" t="s">
         <v>36</v>
@@ -2145,16 +2155,16 @@
       <c r="C12" s="45"/>
       <c r="D12" s="33"/>
       <c r="E12" s="48" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F12" s="33" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G12" s="50" t="s">
         <v>50</v>
       </c>
       <c r="H12" s="33" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I12" s="50"/>
       <c r="J12" s="33"/>
@@ -2162,25 +2172,25 @@
         <v>55</v>
       </c>
       <c r="L12" s="33" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M12" s="50" t="s">
+        <v>63</v>
+      </c>
+      <c r="N12" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="O12" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="N12" s="33" t="s">
+      <c r="P12" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="O12" s="45" t="s">
-        <v>65</v>
-      </c>
-      <c r="P12" s="33" t="s">
-        <v>101</v>
-      </c>
       <c r="Q12" s="50" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="R12" s="33" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="S12" s="62" t="s">
         <v>36</v>
@@ -2197,48 +2207,48 @@
         <v>41</v>
       </c>
       <c r="C13" s="45" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D13" s="33" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E13" s="45" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F13" s="33" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G13" s="50" t="s">
         <v>51</v>
       </c>
       <c r="H13" s="33" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I13" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J13" s="33" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K13" s="21" t="s">
         <v>57</v>
       </c>
       <c r="L13" s="33" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M13" s="48"/>
       <c r="N13" s="33"/>
       <c r="O13" s="45" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="P13" s="33" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="Q13" s="50" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="R13" s="33" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="S13" s="62" t="s">
         <v>36</v>
@@ -2255,10 +2265,10 @@
         <v>42</v>
       </c>
       <c r="C14" s="45" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D14" s="33" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E14" s="45"/>
       <c r="F14" s="33"/>
@@ -2270,7 +2280,7 @@
         <v>58</v>
       </c>
       <c r="J14" s="33" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K14" s="45" t="s">
         <v>36</v>
@@ -2281,10 +2291,10 @@
       <c r="M14" s="48"/>
       <c r="N14" s="33"/>
       <c r="O14" s="45" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="P14" s="33" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="Q14" s="48"/>
       <c r="R14" s="33"/>
@@ -2300,10 +2310,10 @@
         <v>43</v>
       </c>
       <c r="C15" s="45" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E15" s="45"/>
       <c r="F15" s="33"/>
@@ -2317,7 +2327,7 @@
         <v>55</v>
       </c>
       <c r="J15" s="33" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K15" s="45" t="s">
         <v>36</v>
@@ -2376,18 +2386,18 @@
         <v>31</v>
       </c>
       <c r="C17" s="45" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E17" s="51"/>
       <c r="F17" s="33"/>
       <c r="G17" s="48" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H17" s="33" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I17" s="45"/>
       <c r="J17" s="33"/>
@@ -2398,16 +2408,16 @@
       </c>
       <c r="N17" s="33"/>
       <c r="O17" s="48" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="P17" s="33" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="Q17" s="45" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="R17" s="44" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2418,10 +2428,10 @@
         <v>32</v>
       </c>
       <c r="C18" s="45" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D18" s="33" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E18" s="51"/>
       <c r="F18" s="33"/>
@@ -2429,7 +2439,7 @@
         <v>59</v>
       </c>
       <c r="H18" s="33" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I18" s="48"/>
       <c r="J18" s="33"/>
@@ -2442,16 +2452,16 @@
         <v>36</v>
       </c>
       <c r="O18" s="48" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="P18" s="33" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="Q18" s="45" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="R18" s="20" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2462,22 +2472,22 @@
         <v>40</v>
       </c>
       <c r="C19" s="45" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D19" s="33" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E19" s="51" t="s">
         <v>60</v>
       </c>
       <c r="F19" s="33" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G19" s="37" t="s">
         <v>59</v>
       </c>
       <c r="H19" s="33" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I19" s="45"/>
       <c r="J19" s="33"/>
@@ -2492,10 +2502,10 @@
       <c r="O19" s="48"/>
       <c r="P19" s="33"/>
       <c r="Q19" s="45" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="R19" s="33" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:19" ht="80.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2513,7 +2523,7 @@
         <v>60</v>
       </c>
       <c r="F20" s="33" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G20" s="37"/>
       <c r="H20" s="33"/>
@@ -2521,13 +2531,13 @@
         <v>49</v>
       </c>
       <c r="J20" s="33" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K20" s="21" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="L20" s="27" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M20" s="48" t="s">
         <v>36</v>
@@ -2550,24 +2560,24 @@
       <c r="C21" s="47"/>
       <c r="D21" s="33"/>
       <c r="E21" s="21" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F21" s="47" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G21" s="47"/>
       <c r="H21" s="47"/>
       <c r="I21" s="47" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J21" s="20" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K21" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L21" s="33" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="M21" s="48" t="s">
         <v>36</v>
@@ -2590,10 +2600,10 @@
       <c r="C22" s="48"/>
       <c r="D22" s="33"/>
       <c r="E22" s="21" t="s">
-        <v>76</v>
+        <v>109</v>
       </c>
       <c r="F22" s="47" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G22" s="46"/>
       <c r="H22" s="42"/>
@@ -2653,13 +2663,17 @@
       <c r="B24" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="48"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="48" t="s">
+      <c r="C24" s="48" t="s">
         <v>38</v>
       </c>
+      <c r="D24" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>76</v>
+      </c>
       <c r="F24" s="33" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G24" s="51"/>
       <c r="H24" s="33"/>
@@ -2675,20 +2689,24 @@
       <c r="R24" s="34"/>
       <c r="S24" s="41"/>
     </row>
-    <row r="25" spans="1:19" ht="70.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" ht="75.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B25" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="45"/>
-      <c r="D25" s="33"/>
+      <c r="C25" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="33" t="s">
+        <v>104</v>
+      </c>
       <c r="E25" s="48" t="s">
-        <v>44</v>
+        <v>111</v>
       </c>
       <c r="F25" s="33" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G25" s="51"/>
       <c r="H25" s="33"/>
@@ -2703,20 +2721,24 @@
       <c r="Q25" s="52"/>
       <c r="R25" s="28"/>
     </row>
-    <row r="26" spans="1:19" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" ht="105" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B26" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="48"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="48" t="s">
+      <c r="C26" s="48" t="s">
         <v>38</v>
       </c>
+      <c r="D26" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="E26" s="21" t="s">
+        <v>112</v>
+      </c>
       <c r="F26" s="33" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="G26" s="51"/>
       <c r="H26" s="33"/>
@@ -2738,12 +2760,8 @@
       <c r="B27" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="D27" s="44" t="s">
-        <v>106</v>
-      </c>
+      <c r="C27" s="48"/>
+      <c r="D27" s="44"/>
       <c r="E27" s="45" t="s">
         <v>36</v>
       </c>
@@ -2751,10 +2769,10 @@
         <v>36</v>
       </c>
       <c r="G27" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H27" s="33" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I27" s="48"/>
       <c r="J27" s="38"/>
@@ -2774,12 +2792,8 @@
       <c r="B28" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="C28" s="45" t="s">
-        <v>44</v>
-      </c>
-      <c r="D28" s="33" t="s">
-        <v>106</v>
-      </c>
+      <c r="C28" s="45"/>
+      <c r="D28" s="33"/>
       <c r="E28" s="46" t="s">
         <v>36</v>
       </c>
@@ -2787,10 +2801,10 @@
         <v>36</v>
       </c>
       <c r="G28" s="21" t="s">
-        <v>76</v>
+        <v>109</v>
       </c>
       <c r="H28" s="33" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I28" s="42"/>
       <c r="J28" s="20"/>
@@ -2810,12 +2824,8 @@
       <c r="B29" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="C29" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="D29" s="33" t="s">
-        <v>106</v>
-      </c>
+      <c r="C29" s="48"/>
+      <c r="D29" s="33"/>
       <c r="E29" s="42" t="s">
         <v>36</v>
       </c>
@@ -2823,10 +2833,10 @@
         <v>36</v>
       </c>
       <c r="G29" s="21" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H29" s="33" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I29" s="42"/>
       <c r="J29" s="20"/>

</xml_diff>